<commit_message>
new sheet to fill (Brian)
</commit_message>
<xml_diff>
--- a/min20GEEOutput.xlsx
+++ b/min20GEEOutput.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walkermellon/Documents/cav/cancerAcrossVertebrates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walkermellon/cancerAcrossVertebrates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA40074-9506-134B-847E-8C352DACEDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A0854C-2A3E-934A-8FF9-1ECF5CEB3080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40380" yWindow="-18340" windowWidth="27640" windowHeight="16940" xr2:uid="{37396FB1-CC92-E541-BF71-BCE37ABFC157}"/>
+    <workbookView xWindow="2540" yWindow="760" windowWidth="28680" windowHeight="20000" activeTab="1" xr2:uid="{37396FB1-CC92-E541-BF71-BCE37ABFC157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Multivariate" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="Multivariate" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="17">
   <si>
     <t>Neoplasia</t>
   </si>
@@ -83,6 +85,12 @@
   <si>
     <t>note:this is one test per group, not individual regression for each life history variable</t>
   </si>
+  <si>
+    <t>All Species</t>
+  </si>
+  <si>
+    <t>Aves</t>
+  </si>
 </sst>
 </file>
 
@@ -91,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,8 +146,15 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,8 +191,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -369,95 +390,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -825,318 +919,359 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939312B6-DCF3-1B41-AF9A-1FAB66D7BEFF}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="26" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="29"/>
+      <c r="K2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="23"/>
+      <c r="M2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="8"/>
+      <c r="N2" s="25"/>
     </row>
     <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" s="17" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="15">
         <v>1.1529620000000001E-2</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="16">
         <v>0.1763055</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="16">
         <v>7.0686819999999997E-2</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="16">
         <v>-0.5508731</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4" s="16">
         <v>9.8954100000000003E-2</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="17">
         <v>-0.33831050000000001</v>
       </c>
-      <c r="I4" s="37">
+      <c r="I4" s="18">
         <v>5.8833080000000003E-2</v>
       </c>
-      <c r="J4" s="37">
+      <c r="J4" s="18">
         <v>0.1372864</v>
       </c>
-      <c r="K4" s="37">
+      <c r="K4" s="18">
         <v>0.1222796</v>
       </c>
-      <c r="L4" s="37">
+      <c r="L4" s="18">
         <v>-0.52859560000000005</v>
       </c>
-      <c r="M4" s="37">
+      <c r="M4" s="18">
         <v>3.3877409999999997E-2</v>
       </c>
-      <c r="N4" s="38">
+      <c r="N4" s="19">
         <v>-0.46985090000000002</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="41"/>
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="8">
         <v>1.20743997E-2</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="9">
         <v>0.22013740000000001</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="8">
         <v>0.14436660000000001</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="8">
         <v>-0.50047540000000001</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="8">
         <v>9.1952839999999997E-3</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="8">
         <v>-0.70916489999999999</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="8">
         <v>1.470714E-2</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="9">
         <v>0.22606280000000001</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="8">
         <v>0.56834998000000003</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="8">
         <v>0.2140302</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="8">
         <v>8.7248900000000008E-3</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="8">
         <v>-0.75369319999999995</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="41"/>
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="3">
         <v>0.82610570000000005</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="4">
         <v>3.2344310000000001E-2</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="4">
         <v>2.672687E-3</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="4">
         <v>2.0041470000000001</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="4">
         <v>0.1230314</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="4">
         <v>0.65589609999999998</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="4">
         <v>0.97801380000000004</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="4">
         <v>4.5905629999999998E-3</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="4">
         <v>1.0151284700000001E-2</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="4">
         <v>1.8359259999999999</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="4">
         <v>6.7416870000000004E-2</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="4">
         <v>0.90566590000000002</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="41"/>
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="4">
         <v>0.7096481</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="4">
         <v>-0.4213152</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="3">
         <v>2.672687E-3</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="3">
         <v>2.0041470000000001</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="4">
         <v>0.56472370000000005</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="4">
         <v>5.0346989999999998</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="4">
         <v>0.99576819999999999</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="4">
         <v>-6.7885590000000004E-3</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="4">
         <v>1.0151284700000001E-2</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="4">
         <v>1.8359259999999999</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="4">
         <v>0.85118280000000002</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="4">
         <v>-1.891519</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="41"/>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="4">
         <v>0.30054775</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="4">
         <v>-0.23533209999999999</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="3">
         <v>2.672687E-3</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="4">
         <v>2.0041470000000001</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="4">
         <v>0.121048246</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="4">
         <v>1.2017249999999999</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="4">
         <v>3.5569360000000001E-2</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="4">
         <v>0.56331580000000003</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="4">
         <v>1.0151284700000001E-2</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="4">
         <v>1.8359259999999999</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="4">
         <v>0.21311599919999999</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="4">
         <v>0.98427529999999996</v>
       </c>
     </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="41"/>
+      <c r="B9" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="43">
+        <v>0.88490000000000002</v>
+      </c>
+      <c r="D9" s="43">
+        <v>2.7799999999999998E-2</v>
+      </c>
+      <c r="E9" s="43">
+        <v>0.69</v>
+      </c>
+      <c r="F9" s="43">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="G9" s="43">
+        <v>0.65180000000000005</v>
+      </c>
+      <c r="H9" s="43">
+        <v>0.59789999999999999</v>
+      </c>
+      <c r="I9" s="43">
+        <v>0.88439999999999996</v>
+      </c>
+      <c r="J9" s="43">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="K9" s="43">
+        <v>0.73050000000000004</v>
+      </c>
+      <c r="L9" s="43">
+        <v>0.40429999999999999</v>
+      </c>
+      <c r="M9" s="43">
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="N9" s="43">
+        <v>0.67349999999999999</v>
+      </c>
+    </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I25" s="21"/>
+      <c r="I25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A4:A8"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="C1:H1"/>
@@ -1146,13 +1281,14 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A4:A9"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:C8 E8 I4:I8 K7:K8">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="I3:I8 C4:C8 E4:E8 G4:G8 K4:K8 M4:M8">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C8 E4:E8 G4:G8 I3:I8 K4:K8 M4:M8">
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
@@ -1162,11 +1298,390 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39067CE-BE0B-4C43-BB14-675B85B65F29}">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="25"/>
+      <c r="I2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="29"/>
+      <c r="K2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="23"/>
+      <c r="M2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="25"/>
+    </row>
+    <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1.1529620000000001E-2</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.1763055</v>
+      </c>
+      <c r="E4" s="16">
+        <v>7.0686819999999997E-2</v>
+      </c>
+      <c r="F4" s="16">
+        <v>-0.5508731</v>
+      </c>
+      <c r="G4" s="16">
+        <v>9.8954100000000003E-2</v>
+      </c>
+      <c r="H4" s="17">
+        <v>-0.33831050000000001</v>
+      </c>
+      <c r="I4" s="18">
+        <v>5.8833080000000003E-2</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0.1372864</v>
+      </c>
+      <c r="K4" s="18">
+        <v>0.1222796</v>
+      </c>
+      <c r="L4" s="18">
+        <v>-0.52859560000000005</v>
+      </c>
+      <c r="M4" s="18">
+        <v>3.3877409999999997E-2</v>
+      </c>
+      <c r="N4" s="19">
+        <v>-0.46985090000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="41"/>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.20743997E-2</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.22013740000000001</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.14436660000000001</v>
+      </c>
+      <c r="F5" s="8">
+        <v>-0.50047540000000001</v>
+      </c>
+      <c r="G5" s="8">
+        <v>9.1952839999999997E-3</v>
+      </c>
+      <c r="H5" s="8">
+        <v>-0.70916489999999999</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1.470714E-2</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.22606280000000001</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.56834998000000003</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0.2140302</v>
+      </c>
+      <c r="M5" s="8">
+        <v>8.7248900000000008E-3</v>
+      </c>
+      <c r="N5" s="8">
+        <v>-0.75369319999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="41"/>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.82610570000000005</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3.2344310000000001E-2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.672687E-3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2.0041470000000001</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.1230314</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.65589609999999998</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.97801380000000004</v>
+      </c>
+      <c r="J6" s="4">
+        <v>4.5905629999999998E-3</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.0151284700000001E-2</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1.8359259999999999</v>
+      </c>
+      <c r="M6" s="4">
+        <v>6.7416870000000004E-2</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.90566590000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="41"/>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.7096481</v>
+      </c>
+      <c r="D7" s="4">
+        <v>-0.4213152</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.672687E-3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2.0041470000000001</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.56472370000000005</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5.0346989999999998</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.99576819999999999</v>
+      </c>
+      <c r="J7" s="4">
+        <v>-6.7885590000000004E-3</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1.0151284700000001E-2</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1.8359259999999999</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.85118280000000002</v>
+      </c>
+      <c r="N7" s="4">
+        <v>-1.891519</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="41"/>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.30054775</v>
+      </c>
+      <c r="D8" s="4">
+        <v>-0.23533209999999999</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.672687E-3</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2.0041470000000001</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.121048246</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1.2017249999999999</v>
+      </c>
+      <c r="I8" s="4">
+        <v>3.5569360000000001E-2</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.56331580000000003</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1.0151284700000001E-2</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1.8359259999999999</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.21311599919999999</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.98427529999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="41"/>
+      <c r="B9" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="43">
+        <v>0.88490000000000002</v>
+      </c>
+      <c r="D9" s="43">
+        <v>2.7799999999999998E-2</v>
+      </c>
+      <c r="E9" s="43">
+        <v>0.69</v>
+      </c>
+      <c r="F9" s="43">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="G9" s="43">
+        <v>0.65180000000000005</v>
+      </c>
+      <c r="H9" s="43">
+        <v>0.59789999999999999</v>
+      </c>
+      <c r="I9" s="43">
+        <v>0.88439999999999996</v>
+      </c>
+      <c r="J9" s="43">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="K9" s="43">
+        <v>0.73050000000000004</v>
+      </c>
+      <c r="L9" s="43">
+        <v>0.40429999999999999</v>
+      </c>
+      <c r="M9" s="43">
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="N9" s="43">
+        <v>0.67349999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I3:I8 C4:C8 E4:E8 G4:G8 K4:K8 M4:M8">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{684D544E-E3CF-244A-9692-4C05796C9968}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1175,261 +1690,258 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="26"/>
+      <c r="K2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="23"/>
+      <c r="M2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="8"/>
+      <c r="N2" s="25"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" s="17" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="12">
         <v>7.2825679999999997E-3</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="12">
         <v>0.2552856</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="12">
         <v>1.0633851999999999E-2</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="12">
         <v>-0.97792869999999998</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="12">
         <v>0.67639643699999996</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="12">
         <v>-0.1119078</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="12">
         <v>9.4915369999999995E-3</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="12">
         <v>0.26296969999999997</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="12">
         <v>1.9743778E-2</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="12">
         <v>-0.95996950000000003</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="13">
         <v>0.257869448</v>
       </c>
-      <c r="N4" s="31">
+      <c r="N4" s="12">
         <v>-0.33271610000000001</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="12">
         <v>1.8388549999999999E-3</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="12">
         <v>0.35408326000000001</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="12">
         <v>0.96734876199999997</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="12">
         <v>-1.970214E-2</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="12">
         <v>3.858308E-3</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="12">
         <v>-1.1624838099999999</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="12">
         <v>2.2739599999999998E-3</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="12">
         <v>0.3569716</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="12">
         <v>0.13905429999999999</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="13">
         <v>0.78403250000000002</v>
       </c>
-      <c r="M5" s="31">
+      <c r="M5" s="12">
         <v>7.2207029999999997E-5</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="12">
         <v>-1.9210232</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="12">
         <v>2.648408E-2</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="12">
         <v>-0.55530466000000001</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="12">
         <v>0.96653106</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="12">
         <v>-3.6704269999999997E-2</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="12">
         <v>2.035824E-2</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="12">
         <v>1.6894129899999999</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="12">
         <v>4.7669099999999999E-2</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="12">
         <v>-0.5937578</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K6" s="12">
         <v>0.83963633999999998</v>
       </c>
-      <c r="L6" s="31">
+      <c r="L6" s="12">
         <v>-0.22504209999999999</v>
       </c>
-      <c r="M6" s="31">
+      <c r="M6" s="12">
         <v>2.8005789999999999E-2</v>
       </c>
-      <c r="N6" s="31">
+      <c r="N6" s="12">
         <v>1.8863700000000001</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D12" s="24"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1445,13 +1957,139 @@
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="I3:I6 C4:C6 E4:E6 G4:G6 K4:K6 M4:M6">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C6 E4:E6 G4:G6 I4:I6 K4:K6 M4:M6">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7FAC51-6690-CE49-9763-21A7BB84A490}">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+    </row>
+    <row r="2" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="25"/>
+      <c r="G2" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="39"/>
+      <c r="I2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="12">
+        <v>2.1646920000000002E-3</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.29701569999999999</v>
+      </c>
+      <c r="E4" s="12">
+        <v>9.1630439999999997E-4</v>
+      </c>
+      <c r="F4" s="12">
+        <v>-0.99390020000000001</v>
+      </c>
+      <c r="G4" s="12">
+        <v>4.2550400000000002E-2</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.19249939999999999</v>
+      </c>
+      <c r="I4" s="13">
+        <v>1.620898E-3</v>
+      </c>
+      <c r="J4" s="12">
+        <f>--0.9934095</f>
+        <v>0.99340949999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G3:G4 C4 E4 I4">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>